<commit_message>
Latest code from pvt repo
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sukantbhatia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sukantbhatia/Documents/Codes/eclipse-workspace/seleniumAutomation/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A203DB03-09B2-F84D-8CC6-CEA9978F0937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1204E049-AB60-FF45-BD07-739AB2821787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14160" xr2:uid="{BC424CBD-9BB2-C241-B71F-FA85EA03F7D9}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>Mobile Phone</t>
   </si>
   <si>
-    <t>Smart TV</t>
+    <t>Mobiles 5g</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>